<commit_message>
Add Upload Excel Test
</commit_message>
<xml_diff>
--- a/Upload Excel Microservice/src/main/resources/excel.xlsx
+++ b/Upload Excel Microservice/src/main/resources/excel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7F8215B5-3C0B-410F-B2E8-87A81F70B624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C3D51763-DC53-4BA3-A8E7-D13D1553A129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17304" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10668" yWindow="1968" windowWidth="17328" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t xml:space="preserve">  10:30:00</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>BSE</t>
-  </si>
-  <si>
-    <t>asw</t>
   </si>
 </sst>
 </file>
@@ -444,7 +441,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,8 +485,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>

</xml_diff>